<commit_message>
add latex reports and final results
</commit_message>
<xml_diff>
--- a/results/dec_trees/Filetree0.xlsx
+++ b/results/dec_trees/Filetree0.xlsx
@@ -167,10 +167,10 @@
     <t>[2.]</t>
   </si>
   <si>
+    <t>correct</t>
+  </si>
+  <si>
     <t>f1_score</t>
-  </si>
-  <si>
-    <t>correct</t>
   </si>
   <si>
     <t>accuracy</t>
@@ -1405,9 +1405,6 @@
       <c r="A4" t="s">
         <v>41</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1435,7 +1432,7 @@
         <v>49</v>
       </c>
       <c r="B3">
-        <v>0.9180555555555556</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1443,7 +1440,7 @@
         <v>50</v>
       </c>
       <c r="B4">
-        <v>0.92</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1451,7 +1448,7 @@
         <v>51</v>
       </c>
       <c r="B5">
-        <v>0.92</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1536,7 +1533,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1552,7 +1549,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1699,7 +1696,7 @@
         <v>42</v>
       </c>
       <c r="D2">
-        <v>0.52</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1754,7 +1751,7 @@
         <v>7</v>
       </c>
       <c r="D7">
-        <v>0.5600000000000001</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1806,7 +1803,7 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1817,7 +1814,7 @@
         <v>7</v>
       </c>
       <c r="D13">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1870,7 +1867,7 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>0.52</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1884,7 +1881,7 @@
         <v>5</v>
       </c>
       <c r="D18">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1951,7 +1948,7 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1965,7 +1962,7 @@
         <v>5</v>
       </c>
       <c r="D24">
-        <v>0.52</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1979,7 +1976,7 @@
         <v>7</v>
       </c>
       <c r="D25">
-        <v>0.5600000000000001</v>
+        <v>0.52</v>
       </c>
     </row>
   </sheetData>
@@ -2014,7 +2011,7 @@
         <v>42</v>
       </c>
       <c r="D2">
-        <v>0.52</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2069,7 +2066,7 @@
         <v>7</v>
       </c>
       <c r="D7">
-        <v>0.5600000000000001</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2121,7 +2118,7 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2132,7 +2129,7 @@
         <v>7</v>
       </c>
       <c r="D13">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2185,7 +2182,7 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>0.52</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2199,7 +2196,7 @@
         <v>5</v>
       </c>
       <c r="D18">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2266,7 +2263,7 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2280,7 +2277,7 @@
         <v>5</v>
       </c>
       <c r="D24">
-        <v>0.52</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2294,7 +2291,7 @@
         <v>7</v>
       </c>
       <c r="D25">
-        <v>0.5600000000000001</v>
+        <v>0.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>